<commit_message>
Fix TPOT for 40975
</commit_message>
<xml_diff>
--- a/results/multiclass/40975/automl.xlsx
+++ b/results/multiclass/40975/automl.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,6 +504,21 @@
           <t>test_time</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>coverage_error</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>label_ranking_average_precision_score</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>label_ranking_loss</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -576,6 +591,9 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -648,6 +666,9 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -720,6 +741,9 @@
           <t>00:00:09</t>
         </is>
       </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -792,6 +816,9 @@
           <t>00:00:01</t>
         </is>
       </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -864,6 +891,9 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -936,6 +966,9 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1008,6 +1041,9 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1080,6 +1116,9 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1150,6 +1189,96 @@
       <c r="N10" t="inlineStr">
         <is>
           <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>tpot</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0.983</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>-1.000</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0.947</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>0.964</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0.923</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0.983</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0.984</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0.964</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>-1.000</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>-1.000</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>-1.000</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>00:10:10</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>-1.000</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>-1.000</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>-1.000</t>
         </is>
       </c>
     </row>

</xml_diff>